<commit_message>
Important updations on data files for katalon. Separated out all environment data in envtData file and updated all affecting test cases in whole katalon.
</commit_message>
<xml_diff>
--- a/KatalonProjects/credData.xlsx
+++ b/KatalonProjects/credData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>400000002</t>
   </si>
@@ -27,21 +27,12 @@
     <t>blackdress19</t>
   </si>
   <si>
-    <t>https://pushofbiz.cliotest.com/login.php</t>
-  </si>
-  <si>
-    <t>ofbizURL</t>
-  </si>
-  <si>
     <t>ofbizuser</t>
   </si>
   <si>
     <t>ofbizpass</t>
   </si>
   <si>
-    <t>BOURL</t>
-  </si>
-  <si>
     <t>BOuser</t>
   </si>
   <si>
@@ -51,18 +42,12 @@
     <t>CCuser</t>
   </si>
   <si>
-    <t>CCURL</t>
-  </si>
-  <si>
     <t>ehudson</t>
   </si>
   <si>
     <t>CCpass</t>
   </si>
   <si>
-    <t>CWURL</t>
-  </si>
-  <si>
     <t>rsuarez</t>
   </si>
   <si>
@@ -72,9 +57,6 @@
     <t>CWpass</t>
   </si>
   <si>
-    <t>RSURL</t>
-  </si>
-  <si>
     <t>michigan@na.com</t>
   </si>
   <si>
@@ -88,18 +70,6 @@
   </si>
   <si>
     <t>cabiautomation</t>
-  </si>
-  <si>
-    <t>https://sandbox.cabiclio.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://sandbox.cabiclio.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://sandbox.cabiclio.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>https://mirandakate.cabisandbox.com</t>
   </si>
 </sst>
 </file>
@@ -163,12 +133,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -536,125 +505,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="48.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="J2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="C@bi$ush5"/>
-    <hyperlink ref="G2" r:id="rId2" display="https://test17.cliotest.com/cabicentral/control/main"/>
-    <hyperlink ref="J2" r:id="rId3" display="https://test21.cliotest.com/warehouse/control/main"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="M2" r:id="rId5"/>
-    <hyperlink ref="N2" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" display="C@bi$ush5"/>
+    <hyperlink ref="I2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
updated VS_hostess to consider send to stylist button at checkout
</commit_message>
<xml_diff>
--- a/KatalonProjects/credData.xlsx
+++ b/KatalonProjects/credData.xlsx
@@ -72,7 +72,7 @@
     <t>RSemail</t>
   </si>
   <si>
-    <t>vishalguest1@test.com</t>
+    <t>sushantguest1@test.com</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -594,7 +594,7 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="C@bi$ush5"/>
-    <hyperlink ref="I2" r:id="rId2" display="sushantguest1@test.com"/>
+    <hyperlink ref="I2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>